<commit_message>
data exploration section expanded
</commit_message>
<xml_diff>
--- a/TimeSeriesEventData.xlsx
+++ b/TimeSeriesEventData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943E371B-234D-45C4-8044-8F146E993312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E6D5D3-C901-4277-8D8F-3BB5533BC952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F84441A4-1DA5-4DED-9F7A-869C2C707B5F}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{F84441A4-1DA5-4DED-9F7A-869C2C707B5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE943498-6165-45BE-AA33-04F9D689F99E}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A362" workbookViewId="0">
+      <selection activeCell="B368" sqref="B368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3402,12 +3402,8 @@
     </row>
     <row r="368" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A368" s="3"/>
-      <c r="B368" s="4">
-        <v>125</v>
-      </c>
-      <c r="C368" s="4">
-        <v>69</v>
-      </c>
+      <c r="B368" s="4"/>
+      <c r="C368" s="4"/>
     </row>
     <row r="369" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A369" s="3"/>

</xml_diff>